<commit_message>
coded myself into a corner and made some big mistakes, zooming out, have better ideas
</commit_message>
<xml_diff>
--- a/zz Non-LeetCode/HackerRank/Crossword Puzzle/Solution.xlsx
+++ b/zz Non-LeetCode/HackerRank/Crossword Puzzle/Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\zz Non-LeetCode\HackerRank\Crossword Puzzle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7687D426-217B-4710-B619-29E9003102BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A59F46-1191-4F11-846F-6A1D0EDED1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10305" yWindow="2370" windowWidth="10710" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="12">
   <si>
     <t>+</t>
   </si>
@@ -45,6 +45,33 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -60,7 +87,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,6 +97,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -86,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -94,11 +127,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -374,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="I9:AJ42"/>
+  <dimension ref="D9:AQ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="F30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="9:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J17" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="9:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J18" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="9:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J19" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J20" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,7 +748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J21" s="1" t="s">
         <v>0</v>
       </c>
@@ -739,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J22" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J23" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,12 +856,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="9:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:43" x14ac:dyDescent="0.25">
+      <c r="AG26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ26" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="5:43" x14ac:dyDescent="0.25">
       <c r="X27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="AG27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J28" s="1">
         <v>0</v>
       </c>
@@ -848,8 +963,44 @@
       <c r="Y28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="AG28" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="5:43" x14ac:dyDescent="0.25">
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
       <c r="I29" s="1">
         <v>0</v>
       </c>
@@ -886,30 +1037,66 @@
       <c r="X29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="AG29" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="5:43" x14ac:dyDescent="0.25">
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
       <c r="I30" s="1">
         <v>1</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>1</v>
+      <c r="M30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N30" s="2">
+        <v>4</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P30" s="2" t="s">
+      <c r="P30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="Q30" s="1" t="s">
@@ -924,8 +1111,44 @@
       <c r="Y30" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="AG30" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="5:43" x14ac:dyDescent="0.25">
+      <c r="E31" s="1">
+        <v>3</v>
+      </c>
       <c r="I31" s="1">
         <v>2</v>
       </c>
@@ -959,8 +1182,44 @@
       <c r="S31" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="AG31" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="5:43" x14ac:dyDescent="0.25">
+      <c r="E32" s="1">
+        <v>4</v>
+      </c>
       <c r="I32" s="1">
         <v>3</v>
       </c>
@@ -994,8 +1253,41 @@
       <c r="S32" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="9:36" x14ac:dyDescent="0.25">
+      <c r="AG32" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:43" x14ac:dyDescent="0.25">
       <c r="I33" s="1">
         <v>4</v>
       </c>
@@ -1008,19 +1300,19 @@
       <c r="L33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>1</v>
+      <c r="M33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N33" s="2">
+        <v>0</v>
       </c>
       <c r="O33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="2" t="s">
+      <c r="P33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="3" t="s">
         <v>1</v>
       </c>
       <c r="R33" s="1" t="s">
@@ -1029,8 +1321,41 @@
       <c r="S33" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="9:36" x14ac:dyDescent="0.25">
+      <c r="AG33" s="1">
+        <v>7</v>
+      </c>
+      <c r="AH33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:43" x14ac:dyDescent="0.25">
       <c r="I34" s="1">
         <v>5</v>
       </c>
@@ -1043,7 +1368,7 @@
       <c r="L34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="M34" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N34" s="1" t="s">
@@ -1064,8 +1389,41 @@
       <c r="S34" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="9:36" x14ac:dyDescent="0.25">
+      <c r="AG34" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:43" x14ac:dyDescent="0.25">
       <c r="I35" s="1">
         <v>6</v>
       </c>
@@ -1087,8 +1445,8 @@
       <c r="O35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P35" s="2" t="s">
-        <v>1</v>
+      <c r="P35" s="2">
+        <v>3</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>0</v>
@@ -1099,8 +1457,44 @@
       <c r="S35" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="9:36" x14ac:dyDescent="0.25">
+      <c r="AG35" s="1">
+        <v>9</v>
+      </c>
+      <c r="AH35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ35" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
       <c r="I36" s="1">
         <v>7</v>
       </c>
@@ -1135,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="9:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:43" x14ac:dyDescent="0.25">
       <c r="I37" s="1">
         <v>8</v>
       </c>
@@ -1157,7 +1551,7 @@
       <c r="O37" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P37" s="2" t="s">
+      <c r="P37" s="3" t="s">
         <v>1</v>
       </c>
       <c r="Q37" s="1" t="s">
@@ -1170,7 +1564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="9:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:43" x14ac:dyDescent="0.25">
       <c r="I38" s="1">
         <v>9</v>
       </c>
@@ -1205,37 +1599,812 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="9:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1">
+        <v>1</v>
+      </c>
+      <c r="L40" s="1">
+        <v>2</v>
+      </c>
+      <c r="M40" s="1">
+        <v>3</v>
+      </c>
+      <c r="N40" s="1">
+        <v>4</v>
+      </c>
+      <c r="O40" s="1">
+        <v>5</v>
+      </c>
+      <c r="P40" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>7</v>
+      </c>
+      <c r="R40" s="1">
+        <v>8</v>
+      </c>
+      <c r="S40" s="1">
+        <v>9</v>
+      </c>
       <c r="X40" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="9:36" x14ac:dyDescent="0.25">
+      <c r="AD40" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S41" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="X41" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="Z41" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="AA41" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AB41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AF41" s="2" t="s">
+      <c r="AD41" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AI41" s="2" t="s">
+      <c r="AF41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AJ41" s="1" t="s">
+      <c r="AH41" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="9:36" x14ac:dyDescent="0.25">
-      <c r="AF42" s="1" t="s">
+    <row r="42" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="I42" s="1">
+        <v>1</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD42" s="1" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="43" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="I43" s="1">
+        <v>2</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S43" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="I44" s="1">
+        <v>3</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="I45" s="1">
+        <v>4</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="I46" s="1">
+        <v>5</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="I47" s="1">
+        <v>6</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S47" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="I48" s="1">
+        <v>7</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S48" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I49" s="1">
+        <v>8</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S49" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I50" s="1">
+        <v>9</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="J54" s="1">
+        <v>0</v>
+      </c>
+      <c r="K54" s="1">
+        <v>1</v>
+      </c>
+      <c r="L54" s="1">
+        <v>2</v>
+      </c>
+      <c r="M54" s="1">
+        <v>3</v>
+      </c>
+      <c r="N54" s="1">
+        <v>4</v>
+      </c>
+      <c r="O54" s="1">
+        <v>5</v>
+      </c>
+      <c r="P54" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>7</v>
+      </c>
+      <c r="R54" s="1">
+        <v>8</v>
+      </c>
+      <c r="S54" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I55" s="1">
+        <v>0</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I56" s="1">
+        <v>1</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N56" s="1">
+        <v>1</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>2</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S56" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I57" s="1">
+        <v>2</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I58" s="1">
+        <v>3</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M58" s="1">
+        <v>4</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I59" s="1">
+        <v>4</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N59" s="1">
+        <v>0</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S59" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I60" s="1">
+        <v>5</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S60" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I61" s="1">
+        <v>6</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P61" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S61" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I62" s="1">
+        <v>7</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S62" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I63" s="1">
+        <v>8</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S63" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I64" s="1">
+        <v>9</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD49 A50:H64 T50:XFD64 I54:S64 A65:XFD71 A83:XFD1048576 A72:H82 T72:XFD82 I40:S50">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"+"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ironing out recursive loop, about to reconstruct into the 'blacklist' and conventional island method
</commit_message>
<xml_diff>
--- a/zz Non-LeetCode/HackerRank/Crossword Puzzle/Solution.xlsx
+++ b/zz Non-LeetCode/HackerRank/Crossword Puzzle/Solution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\zz Non-LeetCode\HackerRank\Crossword Puzzle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243DDA79-8F7F-4F1C-891B-A5FACA41F4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E14D354-115E-4FFB-8666-0C6550F6751E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="43">
   <si>
     <t>+</t>
   </si>
@@ -102,6 +102,69 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>ORDER</t>
+  </si>
+  <si>
+    <t>for each possibility recurse</t>
+  </si>
+  <si>
+    <t>for each connection, recurse</t>
+  </si>
+  <si>
+    <t>if more slots, recurse on slot</t>
+  </si>
+  <si>
+    <t>recurse</t>
+  </si>
+  <si>
+    <t>slotBank</t>
+  </si>
+  <si>
+    <t>Ignore Visited</t>
+  </si>
+  <si>
+    <t>ignore used words</t>
+  </si>
+  <si>
+    <t>if no more slots, return</t>
+  </si>
+  <si>
+    <t>WORDBANK</t>
+  </si>
+  <si>
+    <t>VISITED</t>
+  </si>
+  <si>
+    <t>PATH</t>
+  </si>
+  <si>
+    <t>if path!=NONE</t>
+  </si>
+  <si>
+    <t>update visited and wordbank</t>
+  </si>
+  <si>
+    <t>visited</t>
+  </si>
+  <si>
+    <t>slotTargetId</t>
+  </si>
+  <si>
+    <t>if no connections,  but there is a slot that isn't visited, return NONE</t>
+  </si>
+  <si>
+    <t>return the call of recurse</t>
+  </si>
+  <si>
+    <t>combine paths</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>path1= the return</t>
   </si>
 </sst>
 </file>
@@ -149,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -160,11 +223,44 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -451,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D9:AR64"/>
+  <dimension ref="D9:AV150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP47" sqref="AP47"/>
+    <sheetView tabSelected="1" topLeftCell="F76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR90" sqref="AR90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,11 +2078,17 @@
       <c r="AI48" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="AJ48" s="1">
+        <v>1</v>
+      </c>
       <c r="AO48" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="49" spans="9:44" x14ac:dyDescent="0.25">
+      <c r="AP48" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I49" s="1">
         <v>8</v>
       </c>
@@ -2023,11 +2125,20 @@
       <c r="AI49" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="AJ49" s="1">
+        <v>2</v>
+      </c>
       <c r="AO49" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="9:44" x14ac:dyDescent="0.25">
+      <c r="AP49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV49" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I50" s="1">
         <v>9</v>
       </c>
@@ -2062,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="9:44" x14ac:dyDescent="0.25">
+    <row r="52" spans="9:48" x14ac:dyDescent="0.25">
       <c r="AE52" s="1" t="s">
         <v>14</v>
       </c>
@@ -2100,16 +2211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="9:44" x14ac:dyDescent="0.25">
-      <c r="Y53" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC53" s="1" t="s">
-        <v>12</v>
-      </c>
+    <row r="53" spans="9:48" x14ac:dyDescent="0.25">
       <c r="AE53" s="1" t="s">
         <v>15</v>
       </c>
@@ -2147,7 +2249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="9:44" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:48" x14ac:dyDescent="0.25">
       <c r="J54" s="1">
         <v>0</v>
       </c>
@@ -2178,15 +2280,6 @@
       <c r="S54" s="1">
         <v>9</v>
       </c>
-      <c r="Y54" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA54" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC54" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="AE54" s="1" t="s">
         <v>16</v>
       </c>
@@ -2224,7 +2317,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="9:44" x14ac:dyDescent="0.25">
+    <row r="55" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I55" s="1">
         <v>0</v>
       </c>
@@ -2258,14 +2351,8 @@
       <c r="S55" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y55" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA55" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="9:44" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I56" s="1">
         <v>1</v>
       </c>
@@ -2299,11 +2386,8 @@
       <c r="S56" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y56" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="9:44" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I57" s="1">
         <v>2</v>
       </c>
@@ -2338,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="9:44" x14ac:dyDescent="0.25">
+    <row r="58" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I58" s="1">
         <v>3</v>
       </c>
@@ -2372,8 +2456,26 @@
       <c r="S58" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="9:44" x14ac:dyDescent="0.25">
+      <c r="Y58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z58" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB58" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I59" s="1">
         <v>4</v>
       </c>
@@ -2407,8 +2509,26 @@
       <c r="S59" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="9:44" x14ac:dyDescent="0.25">
+      <c r="Y59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z59" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB59" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD59" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I60" s="1">
         <v>5</v>
       </c>
@@ -2442,8 +2562,20 @@
       <c r="S60" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="9:44" x14ac:dyDescent="0.25">
+      <c r="Y60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z60" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB60" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I61" s="1">
         <v>6</v>
       </c>
@@ -2477,8 +2609,14 @@
       <c r="S61" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="9:44" x14ac:dyDescent="0.25">
+      <c r="Y61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z61" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I62" s="1">
         <v>7</v>
       </c>
@@ -2513,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="9:44" x14ac:dyDescent="0.25">
+    <row r="63" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I63" s="1">
         <v>8</v>
       </c>
@@ -2548,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="9:44" x14ac:dyDescent="0.25">
+    <row r="64" spans="9:48" x14ac:dyDescent="0.25">
       <c r="I64" s="1">
         <v>9</v>
       </c>
@@ -2583,8 +2721,1032 @@
         <v>0</v>
       </c>
     </row>
+    <row r="77" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="Y77" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z77" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA77" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB77" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC77" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD77" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE77" s="1">
+        <v>6</v>
+      </c>
+      <c r="AF77" s="1">
+        <v>7</v>
+      </c>
+      <c r="AG77" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH77" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="X78" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR78" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="X79" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z79" s="3"/>
+      <c r="AA79" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB79" s="3"/>
+      <c r="AC79" s="2"/>
+      <c r="AD79" s="2"/>
+      <c r="AE79" s="3"/>
+      <c r="AF79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ79" s="3"/>
+      <c r="AK79" s="2"/>
+      <c r="AL79" s="3"/>
+      <c r="AM79" s="2">
+        <v>6</v>
+      </c>
+      <c r="AN79" s="2"/>
+      <c r="AO79" s="3"/>
+      <c r="AP79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR79" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="X80" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB80" s="2"/>
+      <c r="AC80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ80" s="2"/>
+      <c r="AK80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL80" s="2"/>
+      <c r="AM80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR80" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="X81" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB81" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ81" s="2">
+        <v>5</v>
+      </c>
+      <c r="AK81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL81" s="2">
+        <v>7</v>
+      </c>
+      <c r="AM81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR81" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="X82" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB82" s="3"/>
+      <c r="AC82" s="2"/>
+      <c r="AD82" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE82" s="3"/>
+      <c r="AF82" s="3"/>
+      <c r="AG82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ82" s="2"/>
+      <c r="AK82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="3"/>
+      <c r="AM82" s="2">
+        <v>8</v>
+      </c>
+      <c r="AN82" s="2"/>
+      <c r="AO82" s="3"/>
+      <c r="AP82" s="3"/>
+      <c r="AQ82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR82" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="X83" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB83" s="3"/>
+      <c r="AC83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE83" s="2"/>
+      <c r="AF83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ83" s="2"/>
+      <c r="AK83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL83" s="2"/>
+      <c r="AM83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO83" s="2"/>
+      <c r="AP83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR83" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="X84" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE84" s="2">
+        <v>4</v>
+      </c>
+      <c r="AF84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ84" s="3"/>
+      <c r="AK84" s="2"/>
+      <c r="AL84" s="3"/>
+      <c r="AM84" s="2">
+        <v>9</v>
+      </c>
+      <c r="AN84" s="2"/>
+      <c r="AO84" s="2"/>
+      <c r="AP84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR84" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="K85" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X85" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE85" s="2"/>
+      <c r="AF85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO85" s="2">
+        <v>10</v>
+      </c>
+      <c r="AP85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR85" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="L86" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N86" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P86" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X86" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE86" s="3"/>
+      <c r="AF86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO86" s="3"/>
+      <c r="AP86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR86" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="X87" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR87" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="4"/>
+      <c r="S89" s="4"/>
+      <c r="T89" s="4"/>
+      <c r="U89" s="4"/>
+      <c r="V89" s="4"/>
+      <c r="W89" s="4"/>
+      <c r="X89" s="4"/>
+      <c r="Y89" s="4"/>
+      <c r="Z89" s="4"/>
+      <c r="AA89" s="4"/>
+      <c r="AB89" s="4"/>
+      <c r="AC89" s="4"/>
+      <c r="AD89" s="4"/>
+      <c r="AE89" s="4"/>
+      <c r="AF89" s="4"/>
+    </row>
+    <row r="90" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="L90" s="4"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="4"/>
+      <c r="P90" s="4"/>
+      <c r="Q90" s="4"/>
+      <c r="R90" s="4"/>
+      <c r="S90" s="4"/>
+      <c r="T90" s="4"/>
+      <c r="U90" s="4"/>
+      <c r="V90" s="4"/>
+      <c r="W90" s="4"/>
+      <c r="X90" s="4"/>
+      <c r="Y90" s="4"/>
+      <c r="Z90" s="4"/>
+      <c r="AA90" s="4"/>
+      <c r="AB90" s="4"/>
+      <c r="AC90" s="4"/>
+      <c r="AD90" s="4"/>
+      <c r="AE90" s="4"/>
+      <c r="AF90" s="4"/>
+    </row>
+    <row r="91" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="L91" s="1">
+        <v>1</v>
+      </c>
+      <c r="M91" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N91" s="4"/>
+      <c r="O91" s="4"/>
+      <c r="T91" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB91" s="4"/>
+      <c r="AC91" s="4"/>
+      <c r="AD91" s="4"/>
+      <c r="AE91" s="4"/>
+      <c r="AF91" s="4"/>
+    </row>
+    <row r="92" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="M92" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB92" s="4"/>
+      <c r="AC92" s="4"/>
+      <c r="AD92" s="4"/>
+      <c r="AE92" s="4"/>
+      <c r="AF92" s="4"/>
+    </row>
+    <row r="93" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="L93" s="4"/>
+      <c r="AB93" s="4"/>
+      <c r="AC93" s="4"/>
+      <c r="AD93" s="4"/>
+      <c r="AE93" s="4"/>
+      <c r="AF93" s="4"/>
+    </row>
+    <row r="94" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="L94" s="1">
+        <v>1</v>
+      </c>
+      <c r="M94" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB94" s="4"/>
+      <c r="AC94" s="4"/>
+      <c r="AD94" s="4"/>
+      <c r="AE94" s="4"/>
+      <c r="AF94" s="4"/>
+    </row>
+    <row r="95" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="M95" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB95" s="4"/>
+      <c r="AC95" s="4"/>
+      <c r="AD95" s="4"/>
+      <c r="AE95" s="4"/>
+      <c r="AF95" s="4"/>
+    </row>
+    <row r="96" spans="11:44" x14ac:dyDescent="0.25">
+      <c r="M96" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB96" s="4"/>
+      <c r="AC96" s="4"/>
+      <c r="AD96" s="4"/>
+      <c r="AE96" s="4"/>
+      <c r="AF96" s="4"/>
+    </row>
+    <row r="97" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="AB97" s="4"/>
+      <c r="AC97" s="4"/>
+      <c r="AD97" s="4"/>
+      <c r="AE97" s="4"/>
+      <c r="AF97" s="4"/>
+    </row>
+    <row r="98" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="AE98" s="4"/>
+      <c r="AF98" s="4"/>
+    </row>
+    <row r="99" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="M99" s="1">
+        <v>1</v>
+      </c>
+      <c r="N99" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U99" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB99" s="4"/>
+      <c r="AC99" s="4"/>
+      <c r="AD99" s="4"/>
+    </row>
+    <row r="100" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="N100" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA100" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="AC101" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="102" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="L102" s="1">
+        <v>1</v>
+      </c>
+      <c r="M102" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S102" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V102" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA102" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="M103" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S103" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="N107" s="1">
+        <v>2</v>
+      </c>
+      <c r="O107" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+    </row>
+    <row r="108" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="O108" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="N109" s="4"/>
+    </row>
+    <row r="110" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="O110" s="1">
+        <v>2</v>
+      </c>
+      <c r="P110" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="P111" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="P112" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="114" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="P114" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q114" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="115" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="Q115" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="117" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="O117" s="1">
+        <v>2</v>
+      </c>
+      <c r="P117" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="V117" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y117" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA117" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="P118" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="124" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="P124" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q124" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R124" s="4"/>
+      <c r="S124" s="4"/>
+    </row>
+    <row r="125" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="Q125" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="126" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="P126" s="4"/>
+    </row>
+    <row r="127" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="Q127" s="1">
+        <v>3</v>
+      </c>
+      <c r="R127" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="R128" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="129" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="R129" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="R131" s="1">
+        <v>3</v>
+      </c>
+      <c r="S131" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="132" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="S132" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="134" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q134" s="1">
+        <v>3</v>
+      </c>
+      <c r="R134" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="X134" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA134" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC134" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="135" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="R135" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="140" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="R140" s="1">
+        <v>4</v>
+      </c>
+      <c r="S140" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="141" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="R141" s="4"/>
+      <c r="S141" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="143" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="S143" s="1">
+        <v>4</v>
+      </c>
+      <c r="T143" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="T144" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="146" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="T146" s="1">
+        <v>4</v>
+      </c>
+      <c r="U146" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="147" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="U147" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="149" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="R149" s="1">
+        <v>4</v>
+      </c>
+      <c r="S149" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y149" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB149" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD149" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="150" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="S150" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A50:H64 I54:S64 A65:XFD71 A83:XFD1048576 A72:H82 T72:XFD82 I40:S50 T50:AJ50 AL50:XFD50 A1:XFD47 AL48:XFD48 A48:AI48 A49:XFD49 T51:XFD64">
+  <conditionalFormatting sqref="A50:H64 I54:S64 A65:XFD71 A72:H82 T72:XFD76 I40:S50 T50:AJ50 AL50:XFD50 A1:XFD47 AL48:XFD48 A48:AI48 A49:XFD49 T51:XFD52 T53:X56 AD53:XFD56 T57:XFD64 T77:W82 X77:XFD87 A89:XFD90 A88:J88 L88:XFD88 A83:W87 R141 R140:S140 Q135:R135 Q136:Q147 R127:R128 R149:T150 AE123:AF128 AG120:XFD133 AF129:AF134 AE131:AE134 U139:AD143 T135:AD135 T139:T142 X149:AD149 Q134:S134 W134:AC134 Q124:AD124 T125:AD130 P126:P148 P149:Q149 P151:AD151 P150:W150 O118:P118 P110:P111 R118:AB118 O117:Q117 U117:AA117 O107:AB107 R108:AB113 N109:N118 A153:XFD1048576 AE134:XFD152 N152:AD152 N119:O151 AC107:AD114 A91:K102 A103:M152 M94:M95 L102:N102 R102:X102 M91:R91 X91:Z91 T91:V91 P92:Z93 P97:Z97 O94:Y96 Z103 O103:X103 AE98:XFD119 AB100:AD100 L93:L97 L99:L103 AA91:XFD97 AA99:AD99">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"+"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R141">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"+"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V144:Y145 T143:T144">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"+"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V147:Y147">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"+"</formula>
     </cfRule>

</xml_diff>

<commit_message>
single island working on 2 samples
</commit_message>
<xml_diff>
--- a/zz Non-LeetCode/HackerRank/Crossword Puzzle/Solution.xlsx
+++ b/zz Non-LeetCode/HackerRank/Crossword Puzzle/Solution.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\zz Non-LeetCode\HackerRank\Crossword Puzzle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E14D354-115E-4FFB-8666-0C6550F6751E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF12313-B063-477E-A22A-78FB1F9051D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="45">
   <si>
     <t>+</t>
   </si>
@@ -119,9 +119,6 @@
     <t>recurse</t>
   </si>
   <si>
-    <t>slotBank</t>
-  </si>
-  <si>
     <t>Ignore Visited</t>
   </si>
   <si>
@@ -165,6 +162,15 @@
   </si>
   <si>
     <t>path1= the return</t>
+  </si>
+  <si>
+    <t>usedWords</t>
+  </si>
+  <si>
+    <t>mark visited</t>
+  </si>
+  <si>
+    <t>WRONG</t>
   </si>
 </sst>
 </file>
@@ -180,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +205,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -212,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,6 +237,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,6 +291,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -547,10 +570,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="D9:AV150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR90" sqref="AR90"/>
+    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M34" sqref="M30:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3212,13 +3236,13 @@
     </row>
     <row r="86" spans="11:44" x14ac:dyDescent="0.25">
       <c r="L86" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="N86" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P86" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="P86" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="X86" s="1">
         <v>8</v>
@@ -3401,7 +3425,7 @@
       <c r="N91" s="4"/>
       <c r="O91" s="4"/>
       <c r="T91" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AB91" s="4"/>
       <c r="AC91" s="4"/>
@@ -3411,7 +3435,7 @@
     </row>
     <row r="92" spans="11:44" x14ac:dyDescent="0.25">
       <c r="M92" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AB92" s="4"/>
       <c r="AC92" s="4"/>
@@ -3442,7 +3466,7 @@
     </row>
     <row r="95" spans="11:44" x14ac:dyDescent="0.25">
       <c r="M95" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AB95" s="4"/>
       <c r="AC95" s="4"/>
@@ -3451,8 +3475,23 @@
       <c r="AF95" s="4"/>
     </row>
     <row r="96" spans="11:44" x14ac:dyDescent="0.25">
-      <c r="M96" s="4" t="s">
-        <v>38</v>
+      <c r="M96" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
+      <c r="P96" s="6"/>
+      <c r="Q96" s="6"/>
+      <c r="R96" s="6"/>
+      <c r="S96" s="6"/>
+      <c r="T96" s="6"/>
+      <c r="U96" s="6"/>
+      <c r="V96" s="6"/>
+      <c r="W96" s="6"/>
+      <c r="X96" s="6"/>
+      <c r="Y96" s="6"/>
+      <c r="Z96" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="AB96" s="4"/>
       <c r="AC96" s="4"/>
@@ -3476,10 +3515,10 @@
         <v>1</v>
       </c>
       <c r="N99" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U99" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AB99" s="4"/>
       <c r="AC99" s="4"/>
@@ -3487,15 +3526,15 @@
     </row>
     <row r="100" spans="12:32" x14ac:dyDescent="0.25">
       <c r="N100" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA100" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="101" spans="12:32" x14ac:dyDescent="0.25">
       <c r="AC101" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="12:32" x14ac:dyDescent="0.25">
@@ -3503,27 +3542,27 @@
         <v>1</v>
       </c>
       <c r="M102" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S102" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S102" s="1" t="s">
+      <c r="V102" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V102" s="1" t="s">
+      <c r="X102" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="X102" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="AA102" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="103" spans="12:32" x14ac:dyDescent="0.25">
-      <c r="M103" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="104" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="M104" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S103" s="4" t="s">
-        <v>39</v>
+      <c r="S104" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="107" spans="12:32" x14ac:dyDescent="0.25">
@@ -3538,7 +3577,7 @@
     </row>
     <row r="108" spans="12:32" x14ac:dyDescent="0.25">
       <c r="O108" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="109" spans="12:32" x14ac:dyDescent="0.25">
@@ -3554,12 +3593,12 @@
     </row>
     <row r="111" spans="12:32" x14ac:dyDescent="0.25">
       <c r="P111" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="112" spans="12:32" x14ac:dyDescent="0.25">
       <c r="P112" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="114" spans="15:27" x14ac:dyDescent="0.25">
@@ -3567,12 +3606,12 @@
         <v>2</v>
       </c>
       <c r="Q114" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="115" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q115" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="117" spans="15:27" x14ac:dyDescent="0.25">
@@ -3580,16 +3619,16 @@
         <v>2</v>
       </c>
       <c r="P117" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="V117" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V117" s="1" t="s">
+      <c r="Y117" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y117" s="1" t="s">
+      <c r="AA117" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="AA117" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="118" spans="15:27" x14ac:dyDescent="0.25">
@@ -3597,6 +3636,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="123" spans="15:27" x14ac:dyDescent="0.25">
+      <c r="P123" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q123" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="124" spans="15:27" x14ac:dyDescent="0.25">
       <c r="P124" s="1">
         <v>3</v>
@@ -3609,7 +3656,7 @@
     </row>
     <row r="125" spans="15:27" x14ac:dyDescent="0.25">
       <c r="Q125" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="126" spans="15:27" x14ac:dyDescent="0.25">
@@ -3625,12 +3672,12 @@
     </row>
     <row r="128" spans="15:27" x14ac:dyDescent="0.25">
       <c r="R128" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="129" spans="17:29" x14ac:dyDescent="0.25">
       <c r="R129" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="131" spans="17:29" x14ac:dyDescent="0.25">
@@ -3638,12 +3685,12 @@
         <v>3</v>
       </c>
       <c r="S131" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="132" spans="17:29" x14ac:dyDescent="0.25">
       <c r="S132" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="134" spans="17:29" x14ac:dyDescent="0.25">
@@ -3651,20 +3698,20 @@
         <v>3</v>
       </c>
       <c r="R134" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="X134" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="X134" s="1" t="s">
+      <c r="AA134" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AA134" s="1" t="s">
+      <c r="AC134" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AC134" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="135" spans="17:29" x14ac:dyDescent="0.25">
-      <c r="R135" s="4" t="s">
+    </row>
+    <row r="137" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="R137" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3679,7 +3726,7 @@
     <row r="141" spans="17:29" x14ac:dyDescent="0.25">
       <c r="R141" s="4"/>
       <c r="S141" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="143" spans="17:29" x14ac:dyDescent="0.25">
@@ -3692,7 +3739,7 @@
     </row>
     <row r="144" spans="17:29" x14ac:dyDescent="0.25">
       <c r="T144" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="146" spans="18:30" x14ac:dyDescent="0.25">
@@ -3700,12 +3747,12 @@
         <v>4</v>
       </c>
       <c r="U146" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="147" spans="18:30" x14ac:dyDescent="0.25">
       <c r="U147" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="149" spans="18:30" x14ac:dyDescent="0.25">
@@ -3713,16 +3760,16 @@
         <v>4</v>
       </c>
       <c r="S149" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y149" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Y149" s="1" t="s">
+      <c r="AB149" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AB149" s="1" t="s">
+      <c r="AD149" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="AD149" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="150" spans="18:30" x14ac:dyDescent="0.25">
@@ -3731,7 +3778,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A50:H64 I54:S64 A65:XFD71 A72:H82 T72:XFD76 I40:S50 T50:AJ50 AL50:XFD50 A1:XFD47 AL48:XFD48 A48:AI48 A49:XFD49 T51:XFD52 T53:X56 AD53:XFD56 T57:XFD64 T77:W82 X77:XFD87 A89:XFD90 A88:J88 L88:XFD88 A83:W87 R141 R140:S140 Q135:R135 Q136:Q147 R127:R128 R149:T150 AE123:AF128 AG120:XFD133 AF129:AF134 AE131:AE134 U139:AD143 T135:AD135 T139:T142 X149:AD149 Q134:S134 W134:AC134 Q124:AD124 T125:AD130 P126:P148 P149:Q149 P151:AD151 P150:W150 O118:P118 P110:P111 R118:AB118 O117:Q117 U117:AA117 O107:AB107 R108:AB113 N109:N118 A153:XFD1048576 AE134:XFD152 N152:AD152 N119:O151 AC107:AD114 A91:K102 A103:M152 M94:M95 L102:N102 R102:X102 M91:R91 X91:Z91 T91:V91 P92:Z93 P97:Z97 O94:Y96 Z103 O103:X103 AE98:XFD119 AB100:AD100 L93:L97 L99:L103 AA91:XFD97 AA99:AD99">
+  <conditionalFormatting sqref="A50:H64 I54:S64 A65:XFD71 A72:H82 T72:XFD76 I40:S50 T50:AJ50 AL50:XFD50 A1:XFD47 AL48:XFD48 A48:AI48 A49:XFD49 T51:XFD52 T53:X56 AD53:XFD56 T57:XFD64 T77:W82 X77:XFD87 A89:XFD90 A88:J88 L88:XFD88 A83:W87 R141 R140:S140 R127:R128 R149:T150 AE123:AF128 AG120:XFD133 AF129:AF134 AE131:AE134 U139:AD143 T135:AD135 T139:T142 X149:AD149 Q134:S134 W134:AC134 Q124:AD124 T125:AD130 P126:P148 P149:Q149 P151:AD151 P150:W150 O118:P118 P110:P111 R118:AB118 O117:Q117 U117:AA117 O107:AB107 R108:AB113 N109:N118 A153:XFD1048576 AE134:XFD152 N152:AD152 N119:O151 AC107:AD114 A91:K102 M94:M95 L102:N102 R102:X102 M91:R91 X91:Z91 T91:V91 P92:Z93 P97:Z97 O94:Y96 Z103 AE98:XFD119 AB100:AD100 L93:L97 L99:L103 AA91:XFD97 AA99:AD99 Q135:Q147 R137 A103:L103 A104:M152 O103:R103 T103:X103 S104">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"+"</formula>
     </cfRule>

</xml_diff>

<commit_message>
saving excel notes from crossword
</commit_message>
<xml_diff>
--- a/zz Non-LeetCode/HackerRank/Crossword Puzzle/Solution.xlsx
+++ b/zz Non-LeetCode/HackerRank/Crossword Puzzle/Solution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\zz Non-LeetCode\HackerRank\Crossword Puzzle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF12313-B063-477E-A22A-78FB1F9051D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A99EB53-CCD7-4D94-BC6D-54C817B92FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="73">
   <si>
     <t>+</t>
   </si>
@@ -171,6 +171,90 @@
   </si>
   <si>
     <t>WRONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
+  </si>
+  <si>
+    <t>ALMNOP</t>
+  </si>
+  <si>
+    <t>CGHIJK</t>
+  </si>
+  <si>
+    <t>IRSTU</t>
+  </si>
+  <si>
+    <t>TVWXY</t>
+  </si>
+  <si>
+    <t>PQKZEW</t>
   </si>
 </sst>
 </file>
@@ -571,10 +655,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="D9:AV150"/>
+  <dimension ref="D4:AV150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M34" sqref="M30:M34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +668,167 @@
     <col min="25" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="10:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="10:43" x14ac:dyDescent="0.25">
+      <c r="AH4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="10:43" x14ac:dyDescent="0.25">
+      <c r="AH5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="10:43" x14ac:dyDescent="0.25">
+      <c r="AH6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="10:43" x14ac:dyDescent="0.25">
+      <c r="AH7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="10:43" x14ac:dyDescent="0.25">
+      <c r="AH8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="10:43" x14ac:dyDescent="0.25">
       <c r="J9" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,8 +844,102 @@
       <c r="N9" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="10:32" x14ac:dyDescent="0.25">
+      <c r="AH9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="10:43" x14ac:dyDescent="0.25">
+      <c r="AH10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="10:43" x14ac:dyDescent="0.25">
+      <c r="AH11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="10:43" x14ac:dyDescent="0.25">
       <c r="W12" s="1">
         <v>0</v>
       </c>
@@ -632,13 +970,73 @@
       <c r="AF12" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="10:32" x14ac:dyDescent="0.25">
+      <c r="AH12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="10:43" x14ac:dyDescent="0.25">
       <c r="V13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="10:32" x14ac:dyDescent="0.25">
+      <c r="AH13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="10:43" x14ac:dyDescent="0.25">
       <c r="J14" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="10:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="10:43" x14ac:dyDescent="0.25">
       <c r="J15" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +1106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="10:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="10:43" x14ac:dyDescent="0.25">
       <c r="J16" s="1" t="s">
         <v>0</v>
       </c>
@@ -742,6 +1140,36 @@
       <c r="V16" s="1">
         <v>3</v>
       </c>
+      <c r="AH16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK16" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AN16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AO16" s="1">
+        <v>7</v>
+      </c>
+      <c r="AP16" s="1">
+        <v>8</v>
+      </c>
+      <c r="AQ16" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J17" s="1" t="s">
@@ -777,6 +1205,39 @@
       <c r="V17" s="1">
         <v>4</v>
       </c>
+      <c r="AG17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J18" s="1" t="s">
@@ -812,6 +1273,39 @@
       <c r="V18" s="1">
         <v>5</v>
       </c>
+      <c r="AG18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J19" s="1" t="s">
@@ -847,17 +1341,50 @@
       <c r="V19" s="1">
         <v>6</v>
       </c>
-      <c r="AE19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH19" s="2" t="s">
-        <v>1</v>
+      <c r="Z19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="5:43" x14ac:dyDescent="0.25">
@@ -894,8 +1421,41 @@
       <c r="V20" s="1">
         <v>7</v>
       </c>
-      <c r="AE20" s="2" t="s">
-        <v>1</v>
+      <c r="Z20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="5:43" x14ac:dyDescent="0.25">
@@ -932,8 +1492,41 @@
       <c r="V21" s="1">
         <v>8</v>
       </c>
-      <c r="AE21" s="2" t="s">
-        <v>1</v>
+      <c r="Z21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="5:43" x14ac:dyDescent="0.25">
@@ -970,8 +1563,41 @@
       <c r="V22" s="1">
         <v>9</v>
       </c>
-      <c r="AE22" s="2" t="s">
-        <v>1</v>
+      <c r="Z22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG22" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ22" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="5:43" x14ac:dyDescent="0.25">
@@ -1005,10 +1631,113 @@
       <c r="S23" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AG23" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ23" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="5:43" x14ac:dyDescent="0.25">
+      <c r="AG24" s="1">
+        <v>7</v>
+      </c>
+      <c r="AH24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ24" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="5:43" x14ac:dyDescent="0.25">
+      <c r="AG25" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ25" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="5:43" x14ac:dyDescent="0.25">
       <c r="AG26" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AH26" s="1" t="s">
         <v>0</v>
@@ -1045,39 +1774,6 @@
       <c r="X27" s="1">
         <v>1</v>
       </c>
-      <c r="AG27" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ27" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="28" spans="5:43" x14ac:dyDescent="0.25">
       <c r="J28" s="1">
@@ -1113,39 +1809,6 @@
       <c r="Y28" s="1">
         <v>1</v>
       </c>
-      <c r="AG28" s="1">
-        <v>2</v>
-      </c>
-      <c r="AH28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ28" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="29" spans="5:43" x14ac:dyDescent="0.25">
       <c r="E29" s="1">
@@ -1186,39 +1849,6 @@
       </c>
       <c r="X29" s="1">
         <v>1</v>
-      </c>
-      <c r="AG29" s="1">
-        <v>3</v>
-      </c>
-      <c r="AH29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ29" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="30" spans="5:43" x14ac:dyDescent="0.25">
@@ -1238,7 +1868,7 @@
         <v>1</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="N30" s="2">
         <v>1</v>
@@ -1260,39 +1890,6 @@
       </c>
       <c r="Y30" s="1">
         <v>1</v>
-      </c>
-      <c r="AG30" s="1">
-        <v>4</v>
-      </c>
-      <c r="AH30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ30" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="31" spans="5:43" x14ac:dyDescent="0.25">
@@ -1332,38 +1929,8 @@
       <c r="S31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG31" s="1">
-        <v>5</v>
-      </c>
       <c r="AH31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ31" s="1" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="5:43" x14ac:dyDescent="0.25">
@@ -1403,41 +1970,11 @@
       <c r="S32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG32" s="1">
-        <v>6</v>
-      </c>
       <c r="AH32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ32" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="4:43" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I33" s="1">
         <v>4</v>
       </c>
@@ -1471,41 +2008,11 @@
       <c r="S33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG33" s="1">
-        <v>7</v>
-      </c>
       <c r="AH33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ33" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="4:43" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I34" s="1">
         <v>5</v>
       </c>
@@ -1519,7 +2026,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>0</v>
@@ -1539,41 +2046,11 @@
       <c r="S34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG34" s="1">
-        <v>8</v>
-      </c>
       <c r="AH34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ34" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="4:43" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I35" s="1">
         <v>6</v>
       </c>
@@ -1607,41 +2084,11 @@
       <c r="S35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG35" s="1">
-        <v>9</v>
-      </c>
       <c r="AH35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ35" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="4:43" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="4:42" x14ac:dyDescent="0.25">
       <c r="D36" s="1">
         <v>1</v>
       </c>
@@ -1678,8 +2125,11 @@
       <c r="S36" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="4:43" x14ac:dyDescent="0.25">
+      <c r="AH36" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I37" s="1">
         <v>8</v>
       </c>
@@ -1714,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I38" s="1">
         <v>9</v>
       </c>
@@ -1749,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:43" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:42" x14ac:dyDescent="0.25">
       <c r="J40" s="1">
         <v>0</v>
       </c>
@@ -1787,7 +2237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="4:43" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I41" s="1">
         <v>0</v>
       </c>
@@ -1846,7 +2296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="4:43" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I42" s="1">
         <v>1</v>
       </c>
@@ -1887,7 +2337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="4:43" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I43" s="1">
         <v>2</v>
       </c>
@@ -1922,7 +2372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:43" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I44" s="1">
         <v>3</v>
       </c>
@@ -1957,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="4:43" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I45" s="1">
         <v>4</v>
       </c>
@@ -1992,7 +2442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:43" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I46" s="1">
         <v>5</v>
       </c>
@@ -2027,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:43" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I47" s="1">
         <v>6</v>
       </c>
@@ -2065,7 +2515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="4:43" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:42" x14ac:dyDescent="0.25">
       <c r="I48" s="1">
         <v>7</v>
       </c>
@@ -3778,7 +4228,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A50:H64 I54:S64 A65:XFD71 A72:H82 T72:XFD76 I40:S50 T50:AJ50 AL50:XFD50 A1:XFD47 AL48:XFD48 A48:AI48 A49:XFD49 T51:XFD52 T53:X56 AD53:XFD56 T57:XFD64 T77:W82 X77:XFD87 A89:XFD90 A88:J88 L88:XFD88 A83:W87 R141 R140:S140 R127:R128 R149:T150 AE123:AF128 AG120:XFD133 AF129:AF134 AE131:AE134 U139:AD143 T135:AD135 T139:T142 X149:AD149 Q134:S134 W134:AC134 Q124:AD124 T125:AD130 P126:P148 P149:Q149 P151:AD151 P150:W150 O118:P118 P110:P111 R118:AB118 O117:Q117 U117:AA117 O107:AB107 R108:AB113 N109:N118 A153:XFD1048576 AE134:XFD152 N152:AD152 N119:O151 AC107:AD114 A91:K102 M94:M95 L102:N102 R102:X102 M91:R91 X91:Z91 T91:V91 P92:Z93 P97:Z97 O94:Y96 Z103 AE98:XFD119 AB100:AD100 L93:L97 L99:L103 AA91:XFD97 AA99:AD99 Q135:Q147 R137 A103:L103 A104:M152 O103:R103 T103:X103 S104">
+  <conditionalFormatting sqref="A50:H64 I54:S64 A65:XFD71 A72:H82 T72:XFD76 I40:S50 T50:AJ50 AL50:XFD50 AL48:XFD48 A48:AI48 A49:XFD49 T51:XFD52 T53:X56 AD53:XFD56 T57:XFD64 T77:W82 X77:XFD87 A89:XFD90 A88:J88 L88:XFD88 A83:W87 R141 R140:S140 R127:R128 R149:T150 AE123:AF128 AG120:XFD133 AF129:AF134 AE131:AE134 U139:AD143 T135:AD135 T139:T142 X149:AD149 Q134:S134 W134:AC134 Q124:AD124 T125:AD130 P126:P148 P149:Q149 P151:AD151 P150:W150 O118:P118 P110:P111 R118:AB118 O117:Q117 U117:AA117 O107:AB107 R108:AB113 N109:N118 A153:XFD1048576 AE134:XFD152 N152:AD152 N119:O151 AC107:AD114 A91:K102 M94:M95 L102:N102 R102:X102 M91:R91 X91:Z91 T91:V91 P92:Z93 P97:Z97 O94:Y96 Z103 AE98:XFD119 AB100:AD100 L93:L97 L99:L103 AA91:XFD97 AA99:AD99 Q135:Q147 R137 A103:L103 A104:M152 O103:R103 T103:X103 S104 A19:AD22 A36:XFD47 A23:AF35 AR19:XFD35 AG17:AQ26 A1:XFD18">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"+"</formula>
     </cfRule>

</xml_diff>